<commit_message>
Made a few changes to diss
</commit_message>
<xml_diff>
--- a/dissertation/twinpeaks-sa/#twinPeaksData.xlsx
+++ b/dissertation/twinpeaks-sa/#twinPeaksData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\uniWork\dissertation\twinpeaks-sa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB6CE61-F1DF-42A3-987E-8A02DFEA1BAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1650AE3D-A8DB-47CD-80FF-53259A7FFB1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8604" yWindow="2580" windowWidth="17280" windowHeight="8964" xr2:uid="{A2F98D7D-73BE-49C7-AAAC-B193CEB33A64}"/>
+    <workbookView xWindow="5760" yWindow="2496" windowWidth="17280" windowHeight="8964" xr2:uid="{A2F98D7D-73BE-49C7-AAAC-B193CEB33A64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>imdb-rating</t>
   </si>
@@ -74,9 +76,6 @@
   <si>
     <t>bing-neg</t>
   </si>
-  <si>
-    <t>double-check</t>
-  </si>
 </sst>
 </file>
 
@@ -113,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -258,6 +257,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -315,15 +325,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -336,11 +343,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -399,29 +413,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -430,51 +421,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -828,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CCAD1F-C37B-4DA9-8C2A-89122FB84B64}">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:AQ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,11 +800,11 @@
     <col min="11" max="11" width="9.109375" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" style="3" customWidth="1"/>
     <col min="15" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:43" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -890,14 +841,41 @@
       <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="26"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="27"/>
+      <c r="AN1" s="27"/>
+      <c r="AO1" s="27"/>
+      <c r="AP1" s="27"/>
+      <c r="AQ1" s="27"/>
+    </row>
+    <row r="2" spans="1:43" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -928,21 +906,47 @@
       <c r="J2" s="4">
         <v>185</v>
       </c>
-      <c r="K2" s="21">
+      <c r="K2" s="20">
         <v>379</v>
       </c>
       <c r="L2" s="2">
         <v>231</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="4">
         <v>148</v>
       </c>
-      <c r="N2" s="22">
-        <f>L2+M2</f>
-        <v>379</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
+      <c r="AI2" s="27"/>
+      <c r="AJ2" s="27"/>
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
+      <c r="AQ2" s="27"/>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -973,21 +977,47 @@
       <c r="J3" s="4">
         <v>133</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3" s="20">
         <v>270</v>
       </c>
       <c r="L3" s="2">
         <v>154</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="4">
         <v>116</v>
       </c>
-      <c r="N3" s="22">
-        <f t="shared" ref="N3:N49" si="0">L3+M3</f>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="27"/>
+      <c r="AC3" s="27"/>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="27"/>
+      <c r="AF3" s="27"/>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="27"/>
+      <c r="AI3" s="27"/>
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="27"/>
+      <c r="AO3" s="27"/>
+      <c r="AP3" s="27"/>
+      <c r="AQ3" s="27"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1018,21 +1048,47 @@
       <c r="J4" s="4">
         <v>80</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="20">
         <v>168</v>
       </c>
       <c r="L4" s="2">
         <v>98</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="4">
         <v>70</v>
       </c>
-      <c r="N4" s="22">
-        <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="27"/>
+      <c r="AD4" s="27"/>
+      <c r="AE4" s="27"/>
+      <c r="AF4" s="27"/>
+      <c r="AG4" s="27"/>
+      <c r="AH4" s="27"/>
+      <c r="AI4" s="27"/>
+      <c r="AJ4" s="27"/>
+      <c r="AK4" s="27"/>
+      <c r="AL4" s="27"/>
+      <c r="AM4" s="27"/>
+      <c r="AN4" s="27"/>
+      <c r="AO4" s="27"/>
+      <c r="AP4" s="27"/>
+      <c r="AQ4" s="27"/>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1063,21 +1119,47 @@
       <c r="J5" s="4">
         <v>148</v>
       </c>
-      <c r="K5" s="21">
+      <c r="K5" s="20">
         <v>289</v>
       </c>
       <c r="L5" s="2">
         <v>155</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
         <v>134</v>
       </c>
-      <c r="N5" s="22">
-        <f t="shared" si="0"/>
-        <v>289</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="27"/>
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="27"/>
+      <c r="AD5" s="27"/>
+      <c r="AE5" s="27"/>
+      <c r="AF5" s="27"/>
+      <c r="AG5" s="27"/>
+      <c r="AH5" s="27"/>
+      <c r="AI5" s="27"/>
+      <c r="AJ5" s="27"/>
+      <c r="AK5" s="27"/>
+      <c r="AL5" s="27"/>
+      <c r="AM5" s="27"/>
+      <c r="AN5" s="27"/>
+      <c r="AO5" s="27"/>
+      <c r="AP5" s="27"/>
+      <c r="AQ5" s="27"/>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1108,21 +1190,47 @@
       <c r="J6" s="4">
         <v>117</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6" s="20">
         <v>248</v>
       </c>
       <c r="L6" s="2">
         <v>142</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="4">
         <v>106</v>
       </c>
-      <c r="N6" s="22">
-        <f t="shared" si="0"/>
-        <v>248</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+      <c r="AA6" s="27"/>
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="27"/>
+      <c r="AD6" s="27"/>
+      <c r="AE6" s="27"/>
+      <c r="AF6" s="27"/>
+      <c r="AG6" s="27"/>
+      <c r="AH6" s="27"/>
+      <c r="AI6" s="27"/>
+      <c r="AJ6" s="27"/>
+      <c r="AK6" s="27"/>
+      <c r="AL6" s="27"/>
+      <c r="AM6" s="27"/>
+      <c r="AN6" s="27"/>
+      <c r="AO6" s="27"/>
+      <c r="AP6" s="27"/>
+      <c r="AQ6" s="27"/>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1153,21 +1261,47 @@
       <c r="J7" s="4">
         <v>119</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="20">
         <v>251</v>
       </c>
       <c r="L7" s="2">
         <v>138</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="4">
         <v>113</v>
       </c>
-      <c r="N7" s="22">
-        <f t="shared" si="0"/>
-        <v>251</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27"/>
+      <c r="AD7" s="27"/>
+      <c r="AE7" s="27"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
+      <c r="AH7" s="27"/>
+      <c r="AI7" s="27"/>
+      <c r="AJ7" s="27"/>
+      <c r="AK7" s="27"/>
+      <c r="AL7" s="27"/>
+      <c r="AM7" s="27"/>
+      <c r="AN7" s="27"/>
+      <c r="AO7" s="27"/>
+      <c r="AP7" s="27"/>
+      <c r="AQ7" s="27"/>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1198,21 +1332,47 @@
       <c r="J8" s="4">
         <v>86</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="20">
         <v>209</v>
       </c>
       <c r="L8" s="2">
         <v>155</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="4">
         <v>54</v>
       </c>
-      <c r="N8" s="22">
-        <f t="shared" si="0"/>
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="27"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="27"/>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+      <c r="AD8" s="27"/>
+      <c r="AE8" s="27"/>
+      <c r="AF8" s="27"/>
+      <c r="AG8" s="27"/>
+      <c r="AH8" s="27"/>
+      <c r="AI8" s="27"/>
+      <c r="AJ8" s="27"/>
+      <c r="AK8" s="27"/>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="27"/>
+      <c r="AN8" s="27"/>
+      <c r="AO8" s="27"/>
+      <c r="AP8" s="27"/>
+      <c r="AQ8" s="27"/>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>1</v>
       </c>
@@ -1243,22 +1403,48 @@
       <c r="J9" s="7">
         <v>95</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="21">
         <v>178</v>
       </c>
       <c r="L9" s="6">
         <v>94</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="7">
         <v>84</v>
       </c>
-      <c r="N9" s="24">
-        <f t="shared" si="0"/>
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="26">
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="27"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="27"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
+      <c r="AD9" s="27"/>
+      <c r="AE9" s="27"/>
+      <c r="AF9" s="27"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="27"/>
+      <c r="AI9" s="27"/>
+      <c r="AJ9" s="27"/>
+      <c r="AK9" s="27"/>
+      <c r="AL9" s="27"/>
+      <c r="AM9" s="27"/>
+      <c r="AN9" s="27"/>
+      <c r="AO9" s="27"/>
+      <c r="AP9" s="27"/>
+      <c r="AQ9" s="27"/>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A10" s="23">
         <v>2</v>
       </c>
       <c r="B10" s="19">
@@ -1276,7 +1462,7 @@
       <c r="F10" s="19">
         <v>19.100000000000001</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="25">
         <v>93</v>
       </c>
       <c r="H10" s="19">
@@ -1285,7 +1471,7 @@
       <c r="I10" s="19">
         <v>299</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="24">
         <v>164</v>
       </c>
       <c r="K10" s="18">
@@ -1294,15 +1480,41 @@
       <c r="L10" s="19">
         <v>268</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="24">
         <v>174</v>
       </c>
-      <c r="N10" s="20">
-        <f t="shared" si="0"/>
-        <v>442</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
+      <c r="AA10" s="27"/>
+      <c r="AB10" s="27"/>
+      <c r="AC10" s="27"/>
+      <c r="AD10" s="27"/>
+      <c r="AE10" s="27"/>
+      <c r="AF10" s="27"/>
+      <c r="AG10" s="27"/>
+      <c r="AH10" s="27"/>
+      <c r="AI10" s="27"/>
+      <c r="AJ10" s="27"/>
+      <c r="AK10" s="27"/>
+      <c r="AL10" s="27"/>
+      <c r="AM10" s="27"/>
+      <c r="AN10" s="27"/>
+      <c r="AO10" s="27"/>
+      <c r="AP10" s="27"/>
+      <c r="AQ10" s="27"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -1333,21 +1545,47 @@
       <c r="J11" s="4">
         <v>80</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="20">
         <v>187</v>
       </c>
       <c r="L11" s="2">
         <v>106</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="4">
         <v>81</v>
       </c>
-      <c r="N11" s="22">
-        <f t="shared" si="0"/>
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+      <c r="AA11" s="27"/>
+      <c r="AB11" s="27"/>
+      <c r="AC11" s="27"/>
+      <c r="AD11" s="27"/>
+      <c r="AE11" s="27"/>
+      <c r="AF11" s="27"/>
+      <c r="AG11" s="27"/>
+      <c r="AH11" s="27"/>
+      <c r="AI11" s="27"/>
+      <c r="AJ11" s="27"/>
+      <c r="AK11" s="27"/>
+      <c r="AL11" s="27"/>
+      <c r="AM11" s="27"/>
+      <c r="AN11" s="27"/>
+      <c r="AO11" s="27"/>
+      <c r="AP11" s="27"/>
+      <c r="AQ11" s="27"/>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1378,21 +1616,47 @@
       <c r="J12" s="4">
         <v>100</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="20">
         <v>168</v>
       </c>
       <c r="L12" s="2">
         <v>91</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="4">
         <v>77</v>
       </c>
-      <c r="N12" s="22">
-        <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27"/>
+      <c r="AA12" s="27"/>
+      <c r="AB12" s="27"/>
+      <c r="AC12" s="27"/>
+      <c r="AD12" s="27"/>
+      <c r="AE12" s="27"/>
+      <c r="AF12" s="27"/>
+      <c r="AG12" s="27"/>
+      <c r="AH12" s="27"/>
+      <c r="AI12" s="27"/>
+      <c r="AJ12" s="27"/>
+      <c r="AK12" s="27"/>
+      <c r="AL12" s="27"/>
+      <c r="AM12" s="27"/>
+      <c r="AN12" s="27"/>
+      <c r="AO12" s="27"/>
+      <c r="AP12" s="27"/>
+      <c r="AQ12" s="27"/>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -1423,21 +1687,47 @@
       <c r="J13" s="4">
         <v>106</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="20">
         <v>211</v>
       </c>
       <c r="L13" s="2">
         <v>117</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="4">
         <v>94</v>
       </c>
-      <c r="N13" s="22">
-        <f t="shared" si="0"/>
-        <v>211</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27"/>
+      <c r="AA13" s="27"/>
+      <c r="AB13" s="27"/>
+      <c r="AC13" s="27"/>
+      <c r="AD13" s="27"/>
+      <c r="AE13" s="27"/>
+      <c r="AF13" s="27"/>
+      <c r="AG13" s="27"/>
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="27"/>
+      <c r="AJ13" s="27"/>
+      <c r="AK13" s="27"/>
+      <c r="AL13" s="27"/>
+      <c r="AM13" s="27"/>
+      <c r="AN13" s="27"/>
+      <c r="AO13" s="27"/>
+      <c r="AP13" s="27"/>
+      <c r="AQ13" s="27"/>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -1468,21 +1758,47 @@
       <c r="J14" s="4">
         <v>80</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="20">
         <v>180</v>
       </c>
       <c r="L14" s="2">
         <v>105</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="4">
         <v>75</v>
       </c>
-      <c r="N14" s="22">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="27"/>
+      <c r="AE14" s="27"/>
+      <c r="AF14" s="27"/>
+      <c r="AG14" s="27"/>
+      <c r="AH14" s="27"/>
+      <c r="AI14" s="27"/>
+      <c r="AJ14" s="27"/>
+      <c r="AK14" s="27"/>
+      <c r="AL14" s="27"/>
+      <c r="AM14" s="27"/>
+      <c r="AN14" s="27"/>
+      <c r="AO14" s="27"/>
+      <c r="AP14" s="27"/>
+      <c r="AQ14" s="27"/>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -1513,21 +1829,47 @@
       <c r="J15" s="4">
         <v>134</v>
       </c>
-      <c r="K15" s="21">
+      <c r="K15" s="20">
         <v>290</v>
       </c>
       <c r="L15" s="2">
         <v>174</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="4">
         <v>116</v>
       </c>
-      <c r="N15" s="22">
-        <f t="shared" si="0"/>
-        <v>290</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="27"/>
+      <c r="Z15" s="27"/>
+      <c r="AA15" s="27"/>
+      <c r="AB15" s="27"/>
+      <c r="AC15" s="27"/>
+      <c r="AD15" s="27"/>
+      <c r="AE15" s="27"/>
+      <c r="AF15" s="27"/>
+      <c r="AG15" s="27"/>
+      <c r="AH15" s="27"/>
+      <c r="AI15" s="27"/>
+      <c r="AJ15" s="27"/>
+      <c r="AK15" s="27"/>
+      <c r="AL15" s="27"/>
+      <c r="AM15" s="27"/>
+      <c r="AN15" s="27"/>
+      <c r="AO15" s="27"/>
+      <c r="AP15" s="27"/>
+      <c r="AQ15" s="27"/>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -1558,21 +1900,47 @@
       <c r="J16" s="4">
         <v>83</v>
       </c>
-      <c r="K16" s="21">
+      <c r="K16" s="20">
         <v>143</v>
       </c>
       <c r="L16" s="2">
         <v>82</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="4">
         <v>61</v>
       </c>
-      <c r="N16" s="22">
-        <f t="shared" si="0"/>
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="27"/>
+      <c r="AB16" s="27"/>
+      <c r="AC16" s="27"/>
+      <c r="AD16" s="27"/>
+      <c r="AE16" s="27"/>
+      <c r="AF16" s="27"/>
+      <c r="AG16" s="27"/>
+      <c r="AH16" s="27"/>
+      <c r="AI16" s="27"/>
+      <c r="AJ16" s="27"/>
+      <c r="AK16" s="27"/>
+      <c r="AL16" s="27"/>
+      <c r="AM16" s="27"/>
+      <c r="AN16" s="27"/>
+      <c r="AO16" s="27"/>
+      <c r="AP16" s="27"/>
+      <c r="AQ16" s="27"/>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -1603,21 +1971,47 @@
       <c r="J17" s="4">
         <v>128</v>
       </c>
-      <c r="K17" s="21">
+      <c r="K17" s="20">
         <v>258</v>
       </c>
       <c r="L17" s="2">
         <v>149</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="4">
         <v>109</v>
       </c>
-      <c r="N17" s="22">
-        <f t="shared" si="0"/>
-        <v>258</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="27"/>
+      <c r="AA17" s="27"/>
+      <c r="AB17" s="27"/>
+      <c r="AC17" s="27"/>
+      <c r="AD17" s="27"/>
+      <c r="AE17" s="27"/>
+      <c r="AF17" s="27"/>
+      <c r="AG17" s="27"/>
+      <c r="AH17" s="27"/>
+      <c r="AI17" s="27"/>
+      <c r="AJ17" s="27"/>
+      <c r="AK17" s="27"/>
+      <c r="AL17" s="27"/>
+      <c r="AM17" s="27"/>
+      <c r="AN17" s="27"/>
+      <c r="AO17" s="27"/>
+      <c r="AP17" s="27"/>
+      <c r="AQ17" s="27"/>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -1648,21 +2042,47 @@
       <c r="J18" s="4">
         <v>117</v>
       </c>
-      <c r="K18" s="21">
+      <c r="K18" s="20">
         <v>219</v>
       </c>
       <c r="L18" s="2">
         <v>105</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="4">
         <v>114</v>
       </c>
-      <c r="N18" s="22">
-        <f t="shared" si="0"/>
-        <v>219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18" s="27"/>
+      <c r="AA18" s="27"/>
+      <c r="AB18" s="27"/>
+      <c r="AC18" s="27"/>
+      <c r="AD18" s="27"/>
+      <c r="AE18" s="27"/>
+      <c r="AF18" s="27"/>
+      <c r="AG18" s="27"/>
+      <c r="AH18" s="27"/>
+      <c r="AI18" s="27"/>
+      <c r="AJ18" s="27"/>
+      <c r="AK18" s="27"/>
+      <c r="AL18" s="27"/>
+      <c r="AM18" s="27"/>
+      <c r="AN18" s="27"/>
+      <c r="AO18" s="27"/>
+      <c r="AP18" s="27"/>
+      <c r="AQ18" s="27"/>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -1693,21 +2113,47 @@
       <c r="J19" s="4">
         <v>136</v>
       </c>
-      <c r="K19" s="21">
+      <c r="K19" s="20">
         <v>268</v>
       </c>
       <c r="L19" s="2">
         <v>140</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="4">
         <v>128</v>
       </c>
-      <c r="N19" s="22">
-        <f t="shared" si="0"/>
-        <v>268</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27"/>
+      <c r="R19" s="27"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="27"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="27"/>
+      <c r="Y19" s="27"/>
+      <c r="Z19" s="27"/>
+      <c r="AA19" s="27"/>
+      <c r="AB19" s="27"/>
+      <c r="AC19" s="27"/>
+      <c r="AD19" s="27"/>
+      <c r="AE19" s="27"/>
+      <c r="AF19" s="27"/>
+      <c r="AG19" s="27"/>
+      <c r="AH19" s="27"/>
+      <c r="AI19" s="27"/>
+      <c r="AJ19" s="27"/>
+      <c r="AK19" s="27"/>
+      <c r="AL19" s="27"/>
+      <c r="AM19" s="27"/>
+      <c r="AN19" s="27"/>
+      <c r="AO19" s="27"/>
+      <c r="AP19" s="27"/>
+      <c r="AQ19" s="27"/>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -1738,21 +2184,47 @@
       <c r="J20" s="4">
         <v>106</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K20" s="20">
         <v>295</v>
       </c>
       <c r="L20" s="2">
         <v>176</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="4">
         <v>119</v>
       </c>
-      <c r="N20" s="22">
-        <f t="shared" si="0"/>
-        <v>295</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="27"/>
+      <c r="AB20" s="27"/>
+      <c r="AC20" s="27"/>
+      <c r="AD20" s="27"/>
+      <c r="AE20" s="27"/>
+      <c r="AF20" s="27"/>
+      <c r="AG20" s="27"/>
+      <c r="AH20" s="27"/>
+      <c r="AI20" s="27"/>
+      <c r="AJ20" s="27"/>
+      <c r="AK20" s="27"/>
+      <c r="AL20" s="27"/>
+      <c r="AM20" s="27"/>
+      <c r="AN20" s="27"/>
+      <c r="AO20" s="27"/>
+      <c r="AP20" s="27"/>
+      <c r="AQ20" s="27"/>
+    </row>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -1783,21 +2255,47 @@
       <c r="J21" s="4">
         <v>135</v>
       </c>
-      <c r="K21" s="21">
+      <c r="K21" s="20">
         <v>272</v>
       </c>
       <c r="L21" s="2">
         <v>139</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="4">
         <v>133</v>
       </c>
-      <c r="N21" s="22">
-        <f t="shared" si="0"/>
-        <v>272</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="27"/>
+      <c r="AC21" s="27"/>
+      <c r="AD21" s="27"/>
+      <c r="AE21" s="27"/>
+      <c r="AF21" s="27"/>
+      <c r="AG21" s="27"/>
+      <c r="AH21" s="27"/>
+      <c r="AI21" s="27"/>
+      <c r="AJ21" s="27"/>
+      <c r="AK21" s="27"/>
+      <c r="AL21" s="27"/>
+      <c r="AM21" s="27"/>
+      <c r="AN21" s="27"/>
+      <c r="AO21" s="27"/>
+      <c r="AP21" s="27"/>
+      <c r="AQ21" s="27"/>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -1828,21 +2326,47 @@
       <c r="J22" s="4">
         <v>118</v>
       </c>
-      <c r="K22" s="21">
+      <c r="K22" s="20">
         <v>253</v>
       </c>
       <c r="L22" s="2">
         <v>142</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="4">
         <v>111</v>
       </c>
-      <c r="N22" s="22">
-        <f t="shared" si="0"/>
-        <v>253</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27"/>
+      <c r="AA22" s="27"/>
+      <c r="AB22" s="27"/>
+      <c r="AC22" s="27"/>
+      <c r="AD22" s="27"/>
+      <c r="AE22" s="27"/>
+      <c r="AF22" s="27"/>
+      <c r="AG22" s="27"/>
+      <c r="AH22" s="27"/>
+      <c r="AI22" s="27"/>
+      <c r="AJ22" s="27"/>
+      <c r="AK22" s="27"/>
+      <c r="AL22" s="27"/>
+      <c r="AM22" s="27"/>
+      <c r="AN22" s="27"/>
+      <c r="AO22" s="27"/>
+      <c r="AP22" s="27"/>
+      <c r="AQ22" s="27"/>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -1873,21 +2397,47 @@
       <c r="J23" s="4">
         <v>140</v>
       </c>
-      <c r="K23" s="21">
+      <c r="K23" s="20">
         <v>226</v>
       </c>
       <c r="L23" s="2">
         <v>126</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="4">
         <v>100</v>
       </c>
-      <c r="N23" s="22">
-        <f t="shared" si="0"/>
-        <v>226</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="27"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="27"/>
+      <c r="AB23" s="27"/>
+      <c r="AC23" s="27"/>
+      <c r="AD23" s="27"/>
+      <c r="AE23" s="27"/>
+      <c r="AF23" s="27"/>
+      <c r="AG23" s="27"/>
+      <c r="AH23" s="27"/>
+      <c r="AI23" s="27"/>
+      <c r="AJ23" s="27"/>
+      <c r="AK23" s="27"/>
+      <c r="AL23" s="27"/>
+      <c r="AM23" s="27"/>
+      <c r="AN23" s="27"/>
+      <c r="AO23" s="27"/>
+      <c r="AP23" s="27"/>
+      <c r="AQ23" s="27"/>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -1918,21 +2468,47 @@
       <c r="J24" s="4">
         <v>150</v>
       </c>
-      <c r="K24" s="21">
+      <c r="K24" s="20">
         <v>259</v>
       </c>
       <c r="L24" s="2">
         <v>141</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="4">
         <v>118</v>
       </c>
-      <c r="N24" s="22">
-        <f t="shared" si="0"/>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="27"/>
+      <c r="AA24" s="27"/>
+      <c r="AB24" s="27"/>
+      <c r="AC24" s="27"/>
+      <c r="AD24" s="27"/>
+      <c r="AE24" s="27"/>
+      <c r="AF24" s="27"/>
+      <c r="AG24" s="27"/>
+      <c r="AH24" s="27"/>
+      <c r="AI24" s="27"/>
+      <c r="AJ24" s="27"/>
+      <c r="AK24" s="27"/>
+      <c r="AL24" s="27"/>
+      <c r="AM24" s="27"/>
+      <c r="AN24" s="27"/>
+      <c r="AO24" s="27"/>
+      <c r="AP24" s="27"/>
+      <c r="AQ24" s="27"/>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -1963,21 +2539,47 @@
       <c r="J25" s="4">
         <v>140</v>
       </c>
-      <c r="K25" s="21">
+      <c r="K25" s="20">
         <v>283</v>
       </c>
       <c r="L25" s="2">
         <v>147</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="4">
         <v>136</v>
       </c>
-      <c r="N25" s="22">
-        <f t="shared" si="0"/>
-        <v>283</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="27"/>
+      <c r="W25" s="27"/>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="27"/>
+      <c r="AA25" s="27"/>
+      <c r="AB25" s="27"/>
+      <c r="AC25" s="27"/>
+      <c r="AD25" s="27"/>
+      <c r="AE25" s="27"/>
+      <c r="AF25" s="27"/>
+      <c r="AG25" s="27"/>
+      <c r="AH25" s="27"/>
+      <c r="AI25" s="27"/>
+      <c r="AJ25" s="27"/>
+      <c r="AK25" s="27"/>
+      <c r="AL25" s="27"/>
+      <c r="AM25" s="27"/>
+      <c r="AN25" s="27"/>
+      <c r="AO25" s="27"/>
+      <c r="AP25" s="27"/>
+      <c r="AQ25" s="27"/>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -2008,21 +2610,47 @@
       <c r="J26" s="4">
         <v>97</v>
       </c>
-      <c r="K26" s="21">
+      <c r="K26" s="20">
         <v>274</v>
       </c>
       <c r="L26" s="2">
         <v>180</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="4">
         <v>94</v>
       </c>
-      <c r="N26" s="22">
-        <f t="shared" si="0"/>
-        <v>274</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="27"/>
+      <c r="Z26" s="27"/>
+      <c r="AA26" s="27"/>
+      <c r="AB26" s="27"/>
+      <c r="AC26" s="27"/>
+      <c r="AD26" s="27"/>
+      <c r="AE26" s="27"/>
+      <c r="AF26" s="27"/>
+      <c r="AG26" s="27"/>
+      <c r="AH26" s="27"/>
+      <c r="AI26" s="27"/>
+      <c r="AJ26" s="27"/>
+      <c r="AK26" s="27"/>
+      <c r="AL26" s="27"/>
+      <c r="AM26" s="27"/>
+      <c r="AN26" s="27"/>
+      <c r="AO26" s="27"/>
+      <c r="AP26" s="27"/>
+      <c r="AQ26" s="27"/>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -2053,21 +2681,47 @@
       <c r="J27" s="4">
         <v>86</v>
       </c>
-      <c r="K27" s="21">
+      <c r="K27" s="20">
         <v>270</v>
       </c>
       <c r="L27" s="2">
         <v>188</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="4">
         <v>82</v>
       </c>
-      <c r="N27" s="22">
-        <f t="shared" si="0"/>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="27"/>
+      <c r="S27" s="27"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="27"/>
+      <c r="V27" s="27"/>
+      <c r="W27" s="27"/>
+      <c r="X27" s="27"/>
+      <c r="Y27" s="27"/>
+      <c r="Z27" s="27"/>
+      <c r="AA27" s="27"/>
+      <c r="AB27" s="27"/>
+      <c r="AC27" s="27"/>
+      <c r="AD27" s="27"/>
+      <c r="AE27" s="27"/>
+      <c r="AF27" s="27"/>
+      <c r="AG27" s="27"/>
+      <c r="AH27" s="27"/>
+      <c r="AI27" s="27"/>
+      <c r="AJ27" s="27"/>
+      <c r="AK27" s="27"/>
+      <c r="AL27" s="27"/>
+      <c r="AM27" s="27"/>
+      <c r="AN27" s="27"/>
+      <c r="AO27" s="27"/>
+      <c r="AP27" s="27"/>
+      <c r="AQ27" s="27"/>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -2098,21 +2752,47 @@
       <c r="J28" s="4">
         <v>106</v>
       </c>
-      <c r="K28" s="21">
+      <c r="K28" s="20">
         <v>327</v>
       </c>
       <c r="L28" s="2">
         <v>212</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="4">
         <v>115</v>
       </c>
-      <c r="N28" s="22">
-        <f t="shared" si="0"/>
-        <v>327</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="27"/>
+      <c r="S28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="27"/>
+      <c r="V28" s="27"/>
+      <c r="W28" s="27"/>
+      <c r="X28" s="27"/>
+      <c r="Y28" s="27"/>
+      <c r="Z28" s="27"/>
+      <c r="AA28" s="27"/>
+      <c r="AB28" s="27"/>
+      <c r="AC28" s="27"/>
+      <c r="AD28" s="27"/>
+      <c r="AE28" s="27"/>
+      <c r="AF28" s="27"/>
+      <c r="AG28" s="27"/>
+      <c r="AH28" s="27"/>
+      <c r="AI28" s="27"/>
+      <c r="AJ28" s="27"/>
+      <c r="AK28" s="27"/>
+      <c r="AL28" s="27"/>
+      <c r="AM28" s="27"/>
+      <c r="AN28" s="27"/>
+      <c r="AO28" s="27"/>
+      <c r="AP28" s="27"/>
+      <c r="AQ28" s="27"/>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -2143,21 +2823,47 @@
       <c r="J29" s="4">
         <v>120</v>
       </c>
-      <c r="K29" s="21">
+      <c r="K29" s="20">
         <v>268</v>
       </c>
       <c r="L29" s="2">
         <v>144</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="4">
         <v>124</v>
       </c>
-      <c r="N29" s="22">
-        <f t="shared" si="0"/>
-        <v>268</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="27"/>
+      <c r="V29" s="27"/>
+      <c r="W29" s="27"/>
+      <c r="X29" s="27"/>
+      <c r="Y29" s="27"/>
+      <c r="Z29" s="27"/>
+      <c r="AA29" s="27"/>
+      <c r="AB29" s="27"/>
+      <c r="AC29" s="27"/>
+      <c r="AD29" s="27"/>
+      <c r="AE29" s="27"/>
+      <c r="AF29" s="27"/>
+      <c r="AG29" s="27"/>
+      <c r="AH29" s="27"/>
+      <c r="AI29" s="27"/>
+      <c r="AJ29" s="27"/>
+      <c r="AK29" s="27"/>
+      <c r="AL29" s="27"/>
+      <c r="AM29" s="27"/>
+      <c r="AN29" s="27"/>
+      <c r="AO29" s="27"/>
+      <c r="AP29" s="27"/>
+      <c r="AQ29" s="27"/>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -2188,21 +2894,47 @@
       <c r="J30" s="4">
         <v>90</v>
       </c>
-      <c r="K30" s="21">
+      <c r="K30" s="20">
         <v>275</v>
       </c>
       <c r="L30" s="2">
         <v>175</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="4">
         <v>100</v>
       </c>
-      <c r="N30" s="22">
-        <f t="shared" si="0"/>
-        <v>275</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="27"/>
+      <c r="U30" s="27"/>
+      <c r="V30" s="27"/>
+      <c r="W30" s="27"/>
+      <c r="X30" s="27"/>
+      <c r="Y30" s="27"/>
+      <c r="Z30" s="27"/>
+      <c r="AA30" s="27"/>
+      <c r="AB30" s="27"/>
+      <c r="AC30" s="27"/>
+      <c r="AD30" s="27"/>
+      <c r="AE30" s="27"/>
+      <c r="AF30" s="27"/>
+      <c r="AG30" s="27"/>
+      <c r="AH30" s="27"/>
+      <c r="AI30" s="27"/>
+      <c r="AJ30" s="27"/>
+      <c r="AK30" s="27"/>
+      <c r="AL30" s="27"/>
+      <c r="AM30" s="27"/>
+      <c r="AN30" s="27"/>
+      <c r="AO30" s="27"/>
+      <c r="AP30" s="27"/>
+      <c r="AQ30" s="27"/>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>2</v>
       </c>
@@ -2233,21 +2965,47 @@
       <c r="J31" s="7">
         <v>47</v>
       </c>
-      <c r="K31" s="23">
+      <c r="K31" s="21">
         <v>75</v>
       </c>
       <c r="L31" s="6">
         <v>37</v>
       </c>
-      <c r="M31" s="6">
+      <c r="M31" s="7">
         <v>38</v>
       </c>
-      <c r="N31" s="24">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="27"/>
+      <c r="S31" s="27"/>
+      <c r="T31" s="27"/>
+      <c r="U31" s="27"/>
+      <c r="V31" s="27"/>
+      <c r="W31" s="27"/>
+      <c r="X31" s="27"/>
+      <c r="Y31" s="27"/>
+      <c r="Z31" s="27"/>
+      <c r="AA31" s="27"/>
+      <c r="AB31" s="27"/>
+      <c r="AC31" s="27"/>
+      <c r="AD31" s="27"/>
+      <c r="AE31" s="27"/>
+      <c r="AF31" s="27"/>
+      <c r="AG31" s="27"/>
+      <c r="AH31" s="27"/>
+      <c r="AI31" s="27"/>
+      <c r="AJ31" s="27"/>
+      <c r="AK31" s="27"/>
+      <c r="AL31" s="27"/>
+      <c r="AM31" s="27"/>
+      <c r="AN31" s="27"/>
+      <c r="AO31" s="27"/>
+      <c r="AP31" s="27"/>
+      <c r="AQ31" s="27"/>
+    </row>
+    <row r="32" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>3</v>
       </c>
@@ -2266,7 +3024,7 @@
       <c r="F32" s="2">
         <v>0.50600000000000001</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="22">
         <v>59</v>
       </c>
       <c r="H32" s="2">
@@ -2278,21 +3036,47 @@
       <c r="J32" s="4">
         <v>157</v>
       </c>
-      <c r="K32" s="21">
+      <c r="K32" s="20">
         <v>312</v>
       </c>
       <c r="L32" s="2">
         <v>124</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32" s="4">
         <v>188</v>
       </c>
-      <c r="N32" s="22">
-        <f t="shared" si="0"/>
-        <v>312</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N32" s="27"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="27"/>
+      <c r="S32" s="27"/>
+      <c r="T32" s="27"/>
+      <c r="U32" s="27"/>
+      <c r="V32" s="27"/>
+      <c r="W32" s="27"/>
+      <c r="X32" s="27"/>
+      <c r="Y32" s="27"/>
+      <c r="Z32" s="27"/>
+      <c r="AA32" s="27"/>
+      <c r="AB32" s="27"/>
+      <c r="AC32" s="27"/>
+      <c r="AD32" s="27"/>
+      <c r="AE32" s="27"/>
+      <c r="AF32" s="27"/>
+      <c r="AG32" s="27"/>
+      <c r="AH32" s="27"/>
+      <c r="AI32" s="27"/>
+      <c r="AJ32" s="27"/>
+      <c r="AK32" s="27"/>
+      <c r="AL32" s="27"/>
+      <c r="AM32" s="27"/>
+      <c r="AN32" s="27"/>
+      <c r="AO32" s="27"/>
+      <c r="AP32" s="27"/>
+      <c r="AQ32" s="27"/>
+    </row>
+    <row r="33" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -2323,21 +3107,47 @@
       <c r="J33" s="4">
         <v>124</v>
       </c>
-      <c r="K33" s="21">
+      <c r="K33" s="20">
         <v>185</v>
       </c>
       <c r="L33" s="2">
         <v>103</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33" s="4">
         <v>82</v>
       </c>
-      <c r="N33" s="22">
-        <f t="shared" si="0"/>
-        <v>185</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N33" s="27"/>
+      <c r="O33" s="27"/>
+      <c r="P33" s="27"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="27"/>
+      <c r="S33" s="27"/>
+      <c r="T33" s="27"/>
+      <c r="U33" s="27"/>
+      <c r="V33" s="27"/>
+      <c r="W33" s="27"/>
+      <c r="X33" s="27"/>
+      <c r="Y33" s="27"/>
+      <c r="Z33" s="27"/>
+      <c r="AA33" s="27"/>
+      <c r="AB33" s="27"/>
+      <c r="AC33" s="27"/>
+      <c r="AD33" s="27"/>
+      <c r="AE33" s="27"/>
+      <c r="AF33" s="27"/>
+      <c r="AG33" s="27"/>
+      <c r="AH33" s="27"/>
+      <c r="AI33" s="27"/>
+      <c r="AJ33" s="27"/>
+      <c r="AK33" s="27"/>
+      <c r="AL33" s="27"/>
+      <c r="AM33" s="27"/>
+      <c r="AN33" s="27"/>
+      <c r="AO33" s="27"/>
+      <c r="AP33" s="27"/>
+      <c r="AQ33" s="27"/>
+    </row>
+    <row r="34" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>3</v>
       </c>
@@ -2368,21 +3178,47 @@
       <c r="J34" s="4">
         <v>41</v>
       </c>
-      <c r="K34" s="21">
+      <c r="K34" s="20">
         <v>64</v>
       </c>
       <c r="L34" s="2">
         <v>33</v>
       </c>
-      <c r="M34" s="2">
+      <c r="M34" s="4">
         <v>31</v>
       </c>
-      <c r="N34" s="22">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N34" s="27"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="27"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="27"/>
+      <c r="U34" s="27"/>
+      <c r="V34" s="27"/>
+      <c r="W34" s="27"/>
+      <c r="X34" s="27"/>
+      <c r="Y34" s="27"/>
+      <c r="Z34" s="27"/>
+      <c r="AA34" s="27"/>
+      <c r="AB34" s="27"/>
+      <c r="AC34" s="27"/>
+      <c r="AD34" s="27"/>
+      <c r="AE34" s="27"/>
+      <c r="AF34" s="27"/>
+      <c r="AG34" s="27"/>
+      <c r="AH34" s="27"/>
+      <c r="AI34" s="27"/>
+      <c r="AJ34" s="27"/>
+      <c r="AK34" s="27"/>
+      <c r="AL34" s="27"/>
+      <c r="AM34" s="27"/>
+      <c r="AN34" s="27"/>
+      <c r="AO34" s="27"/>
+      <c r="AP34" s="27"/>
+      <c r="AQ34" s="27"/>
+    </row>
+    <row r="35" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>3</v>
       </c>
@@ -2413,21 +3249,47 @@
       <c r="J35" s="4">
         <v>94</v>
       </c>
-      <c r="K35" s="21">
+      <c r="K35" s="20">
         <v>199</v>
       </c>
       <c r="L35" s="2">
         <v>131</v>
       </c>
-      <c r="M35" s="2">
+      <c r="M35" s="4">
         <v>68</v>
       </c>
-      <c r="N35" s="22">
-        <f t="shared" si="0"/>
-        <v>199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N35" s="27"/>
+      <c r="O35" s="27"/>
+      <c r="P35" s="27"/>
+      <c r="Q35" s="27"/>
+      <c r="R35" s="27"/>
+      <c r="S35" s="27"/>
+      <c r="T35" s="27"/>
+      <c r="U35" s="27"/>
+      <c r="V35" s="27"/>
+      <c r="W35" s="27"/>
+      <c r="X35" s="27"/>
+      <c r="Y35" s="27"/>
+      <c r="Z35" s="27"/>
+      <c r="AA35" s="27"/>
+      <c r="AB35" s="27"/>
+      <c r="AC35" s="27"/>
+      <c r="AD35" s="27"/>
+      <c r="AE35" s="27"/>
+      <c r="AF35" s="27"/>
+      <c r="AG35" s="27"/>
+      <c r="AH35" s="27"/>
+      <c r="AI35" s="27"/>
+      <c r="AJ35" s="27"/>
+      <c r="AK35" s="27"/>
+      <c r="AL35" s="27"/>
+      <c r="AM35" s="27"/>
+      <c r="AN35" s="27"/>
+      <c r="AO35" s="27"/>
+      <c r="AP35" s="27"/>
+      <c r="AQ35" s="27"/>
+    </row>
+    <row r="36" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>3</v>
       </c>
@@ -2458,21 +3320,47 @@
       <c r="J36" s="4">
         <v>103</v>
       </c>
-      <c r="K36" s="21">
+      <c r="K36" s="20">
         <v>211</v>
       </c>
       <c r="L36" s="2">
         <v>109</v>
       </c>
-      <c r="M36" s="2">
+      <c r="M36" s="4">
         <v>102</v>
       </c>
-      <c r="N36" s="22">
-        <f t="shared" si="0"/>
-        <v>211</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="27"/>
+      <c r="S36" s="27"/>
+      <c r="T36" s="27"/>
+      <c r="U36" s="27"/>
+      <c r="V36" s="27"/>
+      <c r="W36" s="27"/>
+      <c r="X36" s="27"/>
+      <c r="Y36" s="27"/>
+      <c r="Z36" s="27"/>
+      <c r="AA36" s="27"/>
+      <c r="AB36" s="27"/>
+      <c r="AC36" s="27"/>
+      <c r="AD36" s="27"/>
+      <c r="AE36" s="27"/>
+      <c r="AF36" s="27"/>
+      <c r="AG36" s="27"/>
+      <c r="AH36" s="27"/>
+      <c r="AI36" s="27"/>
+      <c r="AJ36" s="27"/>
+      <c r="AK36" s="27"/>
+      <c r="AL36" s="27"/>
+      <c r="AM36" s="27"/>
+      <c r="AN36" s="27"/>
+      <c r="AO36" s="27"/>
+      <c r="AP36" s="27"/>
+      <c r="AQ36" s="27"/>
+    </row>
+    <row r="37" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>3</v>
       </c>
@@ -2503,21 +3391,47 @@
       <c r="J37" s="4">
         <v>91</v>
       </c>
-      <c r="K37" s="21">
+      <c r="K37" s="20">
         <v>194</v>
       </c>
       <c r="L37" s="2">
         <v>113</v>
       </c>
-      <c r="M37" s="2">
+      <c r="M37" s="4">
         <v>81</v>
       </c>
-      <c r="N37" s="22">
-        <f t="shared" si="0"/>
-        <v>194</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N37" s="27"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="27"/>
+      <c r="S37" s="27"/>
+      <c r="T37" s="27"/>
+      <c r="U37" s="27"/>
+      <c r="V37" s="27"/>
+      <c r="W37" s="27"/>
+      <c r="X37" s="27"/>
+      <c r="Y37" s="27"/>
+      <c r="Z37" s="27"/>
+      <c r="AA37" s="27"/>
+      <c r="AB37" s="27"/>
+      <c r="AC37" s="27"/>
+      <c r="AD37" s="27"/>
+      <c r="AE37" s="27"/>
+      <c r="AF37" s="27"/>
+      <c r="AG37" s="27"/>
+      <c r="AH37" s="27"/>
+      <c r="AI37" s="27"/>
+      <c r="AJ37" s="27"/>
+      <c r="AK37" s="27"/>
+      <c r="AL37" s="27"/>
+      <c r="AM37" s="27"/>
+      <c r="AN37" s="27"/>
+      <c r="AO37" s="27"/>
+      <c r="AP37" s="27"/>
+      <c r="AQ37" s="27"/>
+    </row>
+    <row r="38" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>3</v>
       </c>
@@ -2548,21 +3462,47 @@
       <c r="J38" s="4">
         <v>120</v>
       </c>
-      <c r="K38" s="21">
+      <c r="K38" s="20">
         <v>202</v>
       </c>
       <c r="L38" s="2">
         <v>108</v>
       </c>
-      <c r="M38" s="2">
+      <c r="M38" s="4">
         <v>94</v>
       </c>
-      <c r="N38" s="22">
-        <f t="shared" si="0"/>
-        <v>202</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="27"/>
+      <c r="R38" s="27"/>
+      <c r="S38" s="27"/>
+      <c r="T38" s="27"/>
+      <c r="U38" s="27"/>
+      <c r="V38" s="27"/>
+      <c r="W38" s="27"/>
+      <c r="X38" s="27"/>
+      <c r="Y38" s="27"/>
+      <c r="Z38" s="27"/>
+      <c r="AA38" s="27"/>
+      <c r="AB38" s="27"/>
+      <c r="AC38" s="27"/>
+      <c r="AD38" s="27"/>
+      <c r="AE38" s="27"/>
+      <c r="AF38" s="27"/>
+      <c r="AG38" s="27"/>
+      <c r="AH38" s="27"/>
+      <c r="AI38" s="27"/>
+      <c r="AJ38" s="27"/>
+      <c r="AK38" s="27"/>
+      <c r="AL38" s="27"/>
+      <c r="AM38" s="27"/>
+      <c r="AN38" s="27"/>
+      <c r="AO38" s="27"/>
+      <c r="AP38" s="27"/>
+      <c r="AQ38" s="27"/>
+    </row>
+    <row r="39" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>3</v>
       </c>
@@ -2593,21 +3533,47 @@
       <c r="J39" s="4">
         <v>40</v>
       </c>
-      <c r="K39" s="21">
+      <c r="K39" s="20">
         <v>137</v>
       </c>
       <c r="L39" s="2">
         <v>52</v>
       </c>
-      <c r="M39" s="2">
+      <c r="M39" s="4">
         <v>85</v>
       </c>
-      <c r="N39" s="22">
-        <f t="shared" si="0"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="27"/>
+      <c r="S39" s="27"/>
+      <c r="T39" s="27"/>
+      <c r="U39" s="27"/>
+      <c r="V39" s="27"/>
+      <c r="W39" s="27"/>
+      <c r="X39" s="27"/>
+      <c r="Y39" s="27"/>
+      <c r="Z39" s="27"/>
+      <c r="AA39" s="27"/>
+      <c r="AB39" s="27"/>
+      <c r="AC39" s="27"/>
+      <c r="AD39" s="27"/>
+      <c r="AE39" s="27"/>
+      <c r="AF39" s="27"/>
+      <c r="AG39" s="27"/>
+      <c r="AH39" s="27"/>
+      <c r="AI39" s="27"/>
+      <c r="AJ39" s="27"/>
+      <c r="AK39" s="27"/>
+      <c r="AL39" s="27"/>
+      <c r="AM39" s="27"/>
+      <c r="AN39" s="27"/>
+      <c r="AO39" s="27"/>
+      <c r="AP39" s="27"/>
+      <c r="AQ39" s="27"/>
+    </row>
+    <row r="40" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>3</v>
       </c>
@@ -2638,21 +3604,47 @@
       <c r="J40" s="4">
         <v>98</v>
       </c>
-      <c r="K40" s="21">
+      <c r="K40" s="20">
         <v>191</v>
       </c>
       <c r="L40" s="2">
         <v>104</v>
       </c>
-      <c r="M40" s="2">
+      <c r="M40" s="4">
         <v>87</v>
       </c>
-      <c r="N40" s="22">
-        <f t="shared" si="0"/>
-        <v>191</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27"/>
+      <c r="S40" s="27"/>
+      <c r="T40" s="27"/>
+      <c r="U40" s="27"/>
+      <c r="V40" s="27"/>
+      <c r="W40" s="27"/>
+      <c r="X40" s="27"/>
+      <c r="Y40" s="27"/>
+      <c r="Z40" s="27"/>
+      <c r="AA40" s="27"/>
+      <c r="AB40" s="27"/>
+      <c r="AC40" s="27"/>
+      <c r="AD40" s="27"/>
+      <c r="AE40" s="27"/>
+      <c r="AF40" s="27"/>
+      <c r="AG40" s="27"/>
+      <c r="AH40" s="27"/>
+      <c r="AI40" s="27"/>
+      <c r="AJ40" s="27"/>
+      <c r="AK40" s="27"/>
+      <c r="AL40" s="27"/>
+      <c r="AM40" s="27"/>
+      <c r="AN40" s="27"/>
+      <c r="AO40" s="27"/>
+      <c r="AP40" s="27"/>
+      <c r="AQ40" s="27"/>
+    </row>
+    <row r="41" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>3</v>
       </c>
@@ -2683,21 +3675,47 @@
       <c r="J41" s="4">
         <v>173</v>
       </c>
-      <c r="K41" s="21">
+      <c r="K41" s="20">
         <v>237</v>
       </c>
       <c r="L41" s="2">
         <v>92</v>
       </c>
-      <c r="M41" s="2">
+      <c r="M41" s="4">
         <v>145</v>
       </c>
-      <c r="N41" s="22">
-        <f t="shared" si="0"/>
-        <v>237</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="27"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="27"/>
+      <c r="U41" s="27"/>
+      <c r="V41" s="27"/>
+      <c r="W41" s="27"/>
+      <c r="X41" s="27"/>
+      <c r="Y41" s="27"/>
+      <c r="Z41" s="27"/>
+      <c r="AA41" s="27"/>
+      <c r="AB41" s="27"/>
+      <c r="AC41" s="27"/>
+      <c r="AD41" s="27"/>
+      <c r="AE41" s="27"/>
+      <c r="AF41" s="27"/>
+      <c r="AG41" s="27"/>
+      <c r="AH41" s="27"/>
+      <c r="AI41" s="27"/>
+      <c r="AJ41" s="27"/>
+      <c r="AK41" s="27"/>
+      <c r="AL41" s="27"/>
+      <c r="AM41" s="27"/>
+      <c r="AN41" s="27"/>
+      <c r="AO41" s="27"/>
+      <c r="AP41" s="27"/>
+      <c r="AQ41" s="27"/>
+    </row>
+    <row r="42" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>3</v>
       </c>
@@ -2728,21 +3746,47 @@
       <c r="J42" s="4">
         <v>138</v>
       </c>
-      <c r="K42" s="21">
+      <c r="K42" s="20">
         <v>223</v>
       </c>
       <c r="L42" s="2">
         <v>104</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M42" s="4">
         <v>119</v>
       </c>
-      <c r="N42" s="22">
-        <f t="shared" si="0"/>
-        <v>223</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N42" s="27"/>
+      <c r="O42" s="27"/>
+      <c r="P42" s="27"/>
+      <c r="Q42" s="27"/>
+      <c r="R42" s="27"/>
+      <c r="S42" s="27"/>
+      <c r="T42" s="27"/>
+      <c r="U42" s="27"/>
+      <c r="V42" s="27"/>
+      <c r="W42" s="27"/>
+      <c r="X42" s="27"/>
+      <c r="Y42" s="27"/>
+      <c r="Z42" s="27"/>
+      <c r="AA42" s="27"/>
+      <c r="AB42" s="27"/>
+      <c r="AC42" s="27"/>
+      <c r="AD42" s="27"/>
+      <c r="AE42" s="27"/>
+      <c r="AF42" s="27"/>
+      <c r="AG42" s="27"/>
+      <c r="AH42" s="27"/>
+      <c r="AI42" s="27"/>
+      <c r="AJ42" s="27"/>
+      <c r="AK42" s="27"/>
+      <c r="AL42" s="27"/>
+      <c r="AM42" s="27"/>
+      <c r="AN42" s="27"/>
+      <c r="AO42" s="27"/>
+      <c r="AP42" s="27"/>
+      <c r="AQ42" s="27"/>
+    </row>
+    <row r="43" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>3</v>
       </c>
@@ -2773,21 +3817,47 @@
       <c r="J43" s="4">
         <v>121</v>
       </c>
-      <c r="K43" s="21">
+      <c r="K43" s="20">
         <v>202</v>
       </c>
       <c r="L43" s="2">
         <v>93</v>
       </c>
-      <c r="M43" s="2">
+      <c r="M43" s="4">
         <v>109</v>
       </c>
-      <c r="N43" s="22">
-        <f t="shared" si="0"/>
-        <v>202</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N43" s="27"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="27"/>
+      <c r="Q43" s="27"/>
+      <c r="R43" s="27"/>
+      <c r="S43" s="27"/>
+      <c r="T43" s="27"/>
+      <c r="U43" s="27"/>
+      <c r="V43" s="27"/>
+      <c r="W43" s="27"/>
+      <c r="X43" s="27"/>
+      <c r="Y43" s="27"/>
+      <c r="Z43" s="27"/>
+      <c r="AA43" s="27"/>
+      <c r="AB43" s="27"/>
+      <c r="AC43" s="27"/>
+      <c r="AD43" s="27"/>
+      <c r="AE43" s="27"/>
+      <c r="AF43" s="27"/>
+      <c r="AG43" s="27"/>
+      <c r="AH43" s="27"/>
+      <c r="AI43" s="27"/>
+      <c r="AJ43" s="27"/>
+      <c r="AK43" s="27"/>
+      <c r="AL43" s="27"/>
+      <c r="AM43" s="27"/>
+      <c r="AN43" s="27"/>
+      <c r="AO43" s="27"/>
+      <c r="AP43" s="27"/>
+      <c r="AQ43" s="27"/>
+    </row>
+    <row r="44" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>3</v>
       </c>
@@ -2818,21 +3888,47 @@
       <c r="J44" s="4">
         <v>144</v>
       </c>
-      <c r="K44" s="21">
+      <c r="K44" s="20">
         <v>298</v>
       </c>
       <c r="L44" s="2">
         <v>149</v>
       </c>
-      <c r="M44" s="2">
+      <c r="M44" s="4">
         <v>149</v>
       </c>
-      <c r="N44" s="22">
-        <f t="shared" si="0"/>
-        <v>298</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N44" s="27"/>
+      <c r="O44" s="27"/>
+      <c r="P44" s="27"/>
+      <c r="Q44" s="27"/>
+      <c r="R44" s="27"/>
+      <c r="S44" s="27"/>
+      <c r="T44" s="27"/>
+      <c r="U44" s="27"/>
+      <c r="V44" s="27"/>
+      <c r="W44" s="27"/>
+      <c r="X44" s="27"/>
+      <c r="Y44" s="27"/>
+      <c r="Z44" s="27"/>
+      <c r="AA44" s="27"/>
+      <c r="AB44" s="27"/>
+      <c r="AC44" s="27"/>
+      <c r="AD44" s="27"/>
+      <c r="AE44" s="27"/>
+      <c r="AF44" s="27"/>
+      <c r="AG44" s="27"/>
+      <c r="AH44" s="27"/>
+      <c r="AI44" s="27"/>
+      <c r="AJ44" s="27"/>
+      <c r="AK44" s="27"/>
+      <c r="AL44" s="27"/>
+      <c r="AM44" s="27"/>
+      <c r="AN44" s="27"/>
+      <c r="AO44" s="27"/>
+      <c r="AP44" s="27"/>
+      <c r="AQ44" s="27"/>
+    </row>
+    <row r="45" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>3</v>
       </c>
@@ -2863,21 +3959,47 @@
       <c r="J45" s="4">
         <v>108</v>
       </c>
-      <c r="K45" s="21">
+      <c r="K45" s="20">
         <v>294</v>
       </c>
       <c r="L45" s="2">
         <v>115</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M45" s="4">
         <v>179</v>
       </c>
-      <c r="N45" s="22">
-        <f t="shared" si="0"/>
-        <v>294</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N45" s="27"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="27"/>
+      <c r="Q45" s="27"/>
+      <c r="R45" s="27"/>
+      <c r="S45" s="27"/>
+      <c r="T45" s="27"/>
+      <c r="U45" s="27"/>
+      <c r="V45" s="27"/>
+      <c r="W45" s="27"/>
+      <c r="X45" s="27"/>
+      <c r="Y45" s="27"/>
+      <c r="Z45" s="27"/>
+      <c r="AA45" s="27"/>
+      <c r="AB45" s="27"/>
+      <c r="AC45" s="27"/>
+      <c r="AD45" s="27"/>
+      <c r="AE45" s="27"/>
+      <c r="AF45" s="27"/>
+      <c r="AG45" s="27"/>
+      <c r="AH45" s="27"/>
+      <c r="AI45" s="27"/>
+      <c r="AJ45" s="27"/>
+      <c r="AK45" s="27"/>
+      <c r="AL45" s="27"/>
+      <c r="AM45" s="27"/>
+      <c r="AN45" s="27"/>
+      <c r="AO45" s="27"/>
+      <c r="AP45" s="27"/>
+      <c r="AQ45" s="27"/>
+    </row>
+    <row r="46" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>3</v>
       </c>
@@ -2908,21 +4030,47 @@
       <c r="J46" s="4">
         <v>176</v>
       </c>
-      <c r="K46" s="21">
+      <c r="K46" s="20">
         <v>321</v>
       </c>
       <c r="L46" s="2">
         <v>143</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M46" s="4">
         <v>178</v>
       </c>
-      <c r="N46" s="22">
-        <f t="shared" si="0"/>
-        <v>321</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N46" s="27"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="27"/>
+      <c r="Q46" s="27"/>
+      <c r="R46" s="27"/>
+      <c r="S46" s="27"/>
+      <c r="T46" s="27"/>
+      <c r="U46" s="27"/>
+      <c r="V46" s="27"/>
+      <c r="W46" s="27"/>
+      <c r="X46" s="27"/>
+      <c r="Y46" s="27"/>
+      <c r="Z46" s="27"/>
+      <c r="AA46" s="27"/>
+      <c r="AB46" s="27"/>
+      <c r="AC46" s="27"/>
+      <c r="AD46" s="27"/>
+      <c r="AE46" s="27"/>
+      <c r="AF46" s="27"/>
+      <c r="AG46" s="27"/>
+      <c r="AH46" s="27"/>
+      <c r="AI46" s="27"/>
+      <c r="AJ46" s="27"/>
+      <c r="AK46" s="27"/>
+      <c r="AL46" s="27"/>
+      <c r="AM46" s="27"/>
+      <c r="AN46" s="27"/>
+      <c r="AO46" s="27"/>
+      <c r="AP46" s="27"/>
+      <c r="AQ46" s="27"/>
+    </row>
+    <row r="47" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>3</v>
       </c>
@@ -2953,21 +4101,47 @@
       <c r="J47" s="4">
         <v>95</v>
       </c>
-      <c r="K47" s="21">
+      <c r="K47" s="20">
         <v>177</v>
       </c>
       <c r="L47" s="2">
         <v>87</v>
       </c>
-      <c r="M47" s="2">
+      <c r="M47" s="4">
         <v>90</v>
       </c>
-      <c r="N47" s="22">
-        <f t="shared" si="0"/>
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N47" s="27"/>
+      <c r="O47" s="27"/>
+      <c r="P47" s="27"/>
+      <c r="Q47" s="27"/>
+      <c r="R47" s="27"/>
+      <c r="S47" s="27"/>
+      <c r="T47" s="27"/>
+      <c r="U47" s="27"/>
+      <c r="V47" s="27"/>
+      <c r="W47" s="27"/>
+      <c r="X47" s="27"/>
+      <c r="Y47" s="27"/>
+      <c r="Z47" s="27"/>
+      <c r="AA47" s="27"/>
+      <c r="AB47" s="27"/>
+      <c r="AC47" s="27"/>
+      <c r="AD47" s="27"/>
+      <c r="AE47" s="27"/>
+      <c r="AF47" s="27"/>
+      <c r="AG47" s="27"/>
+      <c r="AH47" s="27"/>
+      <c r="AI47" s="27"/>
+      <c r="AJ47" s="27"/>
+      <c r="AK47" s="27"/>
+      <c r="AL47" s="27"/>
+      <c r="AM47" s="27"/>
+      <c r="AN47" s="27"/>
+      <c r="AO47" s="27"/>
+      <c r="AP47" s="27"/>
+      <c r="AQ47" s="27"/>
+    </row>
+    <row r="48" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>3</v>
       </c>
@@ -2998,21 +4172,47 @@
       <c r="J48" s="4">
         <v>101</v>
       </c>
-      <c r="K48" s="21">
+      <c r="K48" s="20">
         <v>280</v>
       </c>
       <c r="L48" s="2">
         <v>53</v>
       </c>
-      <c r="M48" s="2">
+      <c r="M48" s="4">
         <v>227</v>
       </c>
-      <c r="N48" s="22">
-        <f t="shared" si="0"/>
-        <v>280</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N48" s="27"/>
+      <c r="O48" s="27"/>
+      <c r="P48" s="27"/>
+      <c r="Q48" s="27"/>
+      <c r="R48" s="27"/>
+      <c r="S48" s="27"/>
+      <c r="T48" s="27"/>
+      <c r="U48" s="27"/>
+      <c r="V48" s="27"/>
+      <c r="W48" s="27"/>
+      <c r="X48" s="27"/>
+      <c r="Y48" s="27"/>
+      <c r="Z48" s="27"/>
+      <c r="AA48" s="27"/>
+      <c r="AB48" s="27"/>
+      <c r="AC48" s="27"/>
+      <c r="AD48" s="27"/>
+      <c r="AE48" s="27"/>
+      <c r="AF48" s="27"/>
+      <c r="AG48" s="27"/>
+      <c r="AH48" s="27"/>
+      <c r="AI48" s="27"/>
+      <c r="AJ48" s="27"/>
+      <c r="AK48" s="27"/>
+      <c r="AL48" s="27"/>
+      <c r="AM48" s="27"/>
+      <c r="AN48" s="27"/>
+      <c r="AO48" s="27"/>
+      <c r="AP48" s="27"/>
+      <c r="AQ48" s="27"/>
+    </row>
+    <row r="49" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>3</v>
       </c>
@@ -3043,42 +4243,48 @@
       <c r="J49" s="7">
         <v>50</v>
       </c>
-      <c r="K49" s="23">
+      <c r="K49" s="21">
         <v>78</v>
       </c>
       <c r="L49" s="6">
         <v>21</v>
       </c>
-      <c r="M49" s="6">
+      <c r="M49" s="7">
         <v>57</v>
       </c>
-      <c r="N49" s="24">
-        <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
+      <c r="N49" s="27"/>
+      <c r="O49" s="27"/>
+      <c r="P49" s="27"/>
+      <c r="Q49" s="27"/>
+      <c r="R49" s="27"/>
+      <c r="S49" s="27"/>
+      <c r="T49" s="27"/>
+      <c r="U49" s="27"/>
+      <c r="V49" s="27"/>
+      <c r="W49" s="27"/>
+      <c r="X49" s="27"/>
+      <c r="Y49" s="27"/>
+      <c r="Z49" s="27"/>
+      <c r="AA49" s="27"/>
+      <c r="AB49" s="27"/>
+      <c r="AC49" s="27"/>
+      <c r="AD49" s="27"/>
+      <c r="AE49" s="27"/>
+      <c r="AF49" s="27"/>
+      <c r="AG49" s="27"/>
+      <c r="AH49" s="27"/>
+      <c r="AI49" s="27"/>
+      <c r="AJ49" s="27"/>
+      <c r="AK49" s="27"/>
+      <c r="AL49" s="27"/>
+      <c r="AM49" s="27"/>
+      <c r="AN49" s="27"/>
+      <c r="AO49" s="27"/>
+      <c r="AP49" s="27"/>
+      <c r="AQ49" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="K1:M1">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
-      <formula>"YES"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
-    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576 K1:K1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K9 N2:N9">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10:K31 N10:N31">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32:K49 N32:N49">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added all outputs to Diss
</commit_message>
<xml_diff>
--- a/dissertation/twinpeaks-sa/#twinPeaksData.xlsx
+++ b/dissertation/twinpeaks-sa/#twinPeaksData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\uniWork\dissertation\twinpeaks-sa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CB1028-F8CA-4655-AF47-376288402B20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51FC8AB-399D-4A7D-A8A9-97618FBA8147}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{A2F98D7D-73BE-49C7-AAAC-B193CEB33A64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A2F98D7D-73BE-49C7-AAAC-B193CEB33A64}"/>
   </bookViews>
   <sheets>
     <sheet name="All Data" sheetId="1" r:id="rId1"/>
@@ -349,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -438,9 +438,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -451,11 +448,1838 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="182">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -15798,8 +17622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CCAD1F-C37B-4DA9-8C2A-89122FB84B64}">
   <dimension ref="A1:AQ49"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" activeCellId="1" sqref="C2:D49 E2:E49"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16182,7 +18006,7 @@
       <c r="I5" s="1">
         <v>175</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="35">
         <v>148</v>
       </c>
       <c r="K5" s="4">
@@ -16191,7 +18015,7 @@
       <c r="L5" s="1">
         <v>155</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="35">
         <v>134</v>
       </c>
       <c r="N5" s="1" t="s">
@@ -17802,7 +19626,7 @@
       <c r="I24" s="1">
         <v>154</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="35">
         <v>150</v>
       </c>
       <c r="K24" s="4">
@@ -17882,7 +19706,7 @@
       <c r="L25" s="1">
         <v>147</v>
       </c>
-      <c r="M25" s="19">
+      <c r="M25" s="35">
         <v>136</v>
       </c>
       <c r="N25" s="16" t="s">
@@ -19323,7 +21147,7 @@
       <c r="H44" s="4">
         <v>355</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I44" s="17">
         <v>211</v>
       </c>
       <c r="J44" s="19">
@@ -19619,13 +21443,10 @@
       <c r="L48" s="1">
         <v>53</v>
       </c>
-      <c r="M48" s="19">
+      <c r="M48" s="35">
         <v>227</v>
       </c>
-      <c r="N48" s="6">
-        <f>SUM(L48:M48)</f>
-        <v>280</v>
-      </c>
+      <c r="N48" s="6"/>
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
       <c r="Q48" s="6"/>
@@ -19729,6 +21550,43 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="J10:J31">
+    <cfRule type="top10" dxfId="115" priority="13" rank="10"/>
+    <cfRule type="top10" dxfId="114" priority="11" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J9">
+    <cfRule type="top10" dxfId="113" priority="12" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32:J49">
+    <cfRule type="top10" dxfId="112" priority="10" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I9">
+    <cfRule type="top10" dxfId="111" priority="9" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10:I31">
+    <cfRule type="top10" dxfId="110" priority="8" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32:I49">
+    <cfRule type="top10" dxfId="109" priority="7" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M9">
+    <cfRule type="top10" dxfId="108" priority="6" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M10:M31">
+    <cfRule type="top10" dxfId="107" priority="5" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M32:M49">
+    <cfRule type="top10" dxfId="106" priority="4" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L9">
+    <cfRule type="top10" dxfId="105" priority="3" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L10:L31">
+    <cfRule type="top10" dxfId="104" priority="2" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L32:L49">
+    <cfRule type="top10" dxfId="91" priority="1" rank="3"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
@@ -19741,8 +21599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0798C36F-CFC8-4190-A3BF-F9AF6628BE09}">
   <dimension ref="B2:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20309,6 +22167,31 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D35:D52">
+    <cfRule type="top10" dxfId="0" priority="13" percent="1" rank="2"/>
+    <cfRule type="top10" dxfId="1" priority="11" rank="3"/>
+    <cfRule type="top10" dxfId="2" priority="1" bottom="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C52">
+    <cfRule type="top10" dxfId="24" priority="12" rank="3"/>
+    <cfRule type="top10" dxfId="23" priority="2" bottom="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D10">
+    <cfRule type="top10" dxfId="22" priority="10" rank="3"/>
+    <cfRule type="top10" dxfId="21" priority="3" bottom="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C10">
+    <cfRule type="top10" dxfId="20" priority="9" rank="3"/>
+    <cfRule type="top10" dxfId="19" priority="4" bottom="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:C33">
+    <cfRule type="top10" dxfId="18" priority="8" rank="3"/>
+    <cfRule type="top10" dxfId="17" priority="6" bottom="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D33">
+    <cfRule type="top10" dxfId="16" priority="7" rank="3"/>
+    <cfRule type="top10" dxfId="15" priority="5" bottom="1" rank="3"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -21483,47 +23366,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="31"/>
-    <col min="2" max="2" width="13.88671875" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="31"/>
+    <col min="1" max="1" width="8.88671875" style="30"/>
+    <col min="2" max="2" width="13.88671875" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="29" t="s">
@@ -21538,688 +23421,688 @@
       <c r="E5" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="30" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <v>34.6</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <v>8.9</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <v>10</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <v>23.2</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <v>8.4</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <v>10</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <v>19.2</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>9</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>8.6</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="32">
+      <c r="B9" s="31">
         <v>16.7</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="31">
         <v>8.4</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <v>8.6</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>17.399999999999999</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <v>7.1</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="32">
+      <c r="B11" s="31">
         <v>17.3</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="31">
         <v>8.6</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <v>8.6</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="32">
+      <c r="B12" s="31">
         <v>15.6</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="31">
         <v>8.6</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="31">
         <v>7.1</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <v>18.7</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="32">
         <v>9.1</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="32">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="32">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="33">
         <v>19.100000000000001</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="33">
         <v>9</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="33">
         <v>10</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="33">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="32">
+      <c r="B15" s="31">
         <v>14.4</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="31">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="31">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="31">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="32">
+      <c r="B16" s="31">
         <v>13.7</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="31">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="31">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="32">
+      <c r="B17" s="31">
         <v>12.8</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <v>6.7</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="31">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="32">
+      <c r="B18" s="31">
         <v>11.4</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="31">
         <v>8.5</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <v>6.7</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="31">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="32">
+      <c r="B19" s="31">
         <v>11.3</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <v>8.6</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="31">
         <v>10</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="31">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="32">
+      <c r="B20" s="31">
         <v>17.2</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <v>9.4</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="31">
         <v>10</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="31">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="32">
+      <c r="B21" s="31">
         <v>13.3</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <v>8.6</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="31">
         <v>6.7</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="31">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="32">
+      <c r="B22" s="31">
         <v>12.4</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <v>9.3000000000000007</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="31">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="31">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="32">
+      <c r="B23" s="31">
         <v>11.1</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="31">
         <v>7.9</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="31">
         <v>5</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="31">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="32">
+      <c r="B24" s="31">
         <v>12.1</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="31">
         <v>7.5</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <v>5</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="31">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="32">
+      <c r="B25" s="31">
         <v>10.3</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="31">
         <v>7.6</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="31">
         <v>4</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="32">
+      <c r="B26" s="31">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="31">
         <v>7.8</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="31">
         <v>6</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="32">
+      <c r="B27" s="31">
         <v>8.6999999999999993</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="31">
         <v>7.7</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="31">
         <v>6</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="32">
+      <c r="B28" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="31">
         <v>7.5</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="31">
         <v>2</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="32">
+      <c r="B29" s="31">
         <v>7.8</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="31">
         <v>7.9</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="31">
         <v>4</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="32">
+      <c r="B30" s="31">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="31">
         <v>7.6</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="31">
         <v>8</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="32">
+      <c r="B31" s="31">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="31">
         <v>8.1</v>
       </c>
-      <c r="D31" s="32">
+      <c r="D31" s="31">
         <v>10</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="32">
+      <c r="B32" s="31">
         <v>7.9</v>
       </c>
-      <c r="C32" s="32">
+      <c r="C32" s="31">
         <v>8.1</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="31">
         <v>10</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="32">
+      <c r="B33" s="31">
         <v>7.4</v>
       </c>
-      <c r="C33" s="32">
+      <c r="C33" s="31">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="31">
         <v>10</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="32">
+      <c r="B34" s="31">
         <v>10.4</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="31">
         <v>8.6</v>
       </c>
-      <c r="D34" s="32">
+      <c r="D34" s="31">
         <v>10</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="33">
+      <c r="B35" s="32">
         <v>10.4</v>
       </c>
-      <c r="C35" s="33">
+      <c r="C35" s="32">
         <v>9.3000000000000007</v>
       </c>
-      <c r="D35" s="33">
+      <c r="D35" s="32">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E35" s="33">
+      <c r="E35" s="32">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="32">
+      <c r="B36" s="31">
         <v>0.50600000000000001</v>
       </c>
-      <c r="C36" s="32">
+      <c r="C36" s="31">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D36" s="32">
+      <c r="D36" s="31">
         <v>10</v>
       </c>
-      <c r="E36" s="32">
+      <c r="E36" s="31">
         <v>2.9</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="32">
+      <c r="B37" s="31">
         <v>0.50600000000000001</v>
       </c>
-      <c r="C37" s="32">
+      <c r="C37" s="31">
         <v>8.8000000000000007</v>
       </c>
-      <c r="D37" s="32">
+      <c r="D37" s="31">
         <v>10</v>
       </c>
-      <c r="E37" s="32">
+      <c r="E37" s="31">
         <v>1.3</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="32">
+      <c r="B38" s="31">
         <v>0.19500000000000001</v>
       </c>
-      <c r="C38" s="32">
+      <c r="C38" s="31">
         <v>8.5</v>
       </c>
-      <c r="D38" s="32">
+      <c r="D38" s="31">
         <v>10</v>
       </c>
-      <c r="E38" s="32">
+      <c r="E38" s="31">
         <v>2.1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="32">
+      <c r="B39" s="31">
         <v>0.19500000000000001</v>
       </c>
-      <c r="C39" s="32">
+      <c r="C39" s="31">
         <v>8.6</v>
       </c>
-      <c r="D39" s="32">
+      <c r="D39" s="31">
         <v>10</v>
       </c>
-      <c r="E39" s="32">
+      <c r="E39" s="31">
         <v>1.4</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="32">
+      <c r="B40" s="31">
         <v>0.254</v>
       </c>
-      <c r="C40" s="32">
+      <c r="C40" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D40" s="32">
+      <c r="D40" s="31">
         <v>10</v>
       </c>
-      <c r="E40" s="32">
+      <c r="E40" s="31">
         <v>1.5</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="32">
+      <c r="B41" s="31">
         <v>0.27</v>
       </c>
-      <c r="C41" s="32">
+      <c r="C41" s="31">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D41" s="32">
+      <c r="D41" s="31">
         <v>10</v>
       </c>
-      <c r="E41" s="32">
+      <c r="E41" s="31">
         <v>1.9</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="32">
+      <c r="B42" s="31">
         <v>0.29399999999999998</v>
       </c>
-      <c r="C42" s="32">
+      <c r="C42" s="31">
         <v>8.8000000000000007</v>
       </c>
-      <c r="D42" s="32">
+      <c r="D42" s="31">
         <v>10</v>
       </c>
-      <c r="E42" s="32">
+      <c r="E42" s="31">
         <v>1.5</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B43" s="32">
+      <c r="B43" s="31">
         <v>0.246</v>
       </c>
-      <c r="C43" s="32">
+      <c r="C43" s="31">
         <v>8.8000000000000007</v>
       </c>
-      <c r="D43" s="32">
+      <c r="D43" s="31">
         <v>10</v>
       </c>
-      <c r="E43" s="32">
+      <c r="E43" s="31">
         <v>2.8</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="32">
+      <c r="B44" s="31">
         <v>0.35499999999999998</v>
       </c>
-      <c r="C44" s="32">
+      <c r="C44" s="31">
         <v>8.5</v>
       </c>
-      <c r="D44" s="32">
+      <c r="D44" s="31">
         <v>10</v>
       </c>
-      <c r="E44" s="32">
+      <c r="E44" s="31">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="32">
+      <c r="B45" s="31">
         <v>0.26700000000000002</v>
       </c>
-      <c r="C45" s="32">
+      <c r="C45" s="31">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D45" s="32">
+      <c r="D45" s="31">
         <v>10</v>
       </c>
-      <c r="E45" s="32">
+      <c r="E45" s="31">
         <v>1.7</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="32">
+      <c r="B46" s="31">
         <v>0.219</v>
       </c>
-      <c r="C46" s="32">
+      <c r="C46" s="31">
         <v>9</v>
       </c>
-      <c r="D46" s="32">
+      <c r="D46" s="31">
         <v>10</v>
       </c>
-      <c r="E46" s="32">
+      <c r="E46" s="31">
         <v>1.6</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="32">
+      <c r="B47" s="31">
         <v>0.24</v>
       </c>
-      <c r="C47" s="32">
+      <c r="C47" s="31">
         <v>7.8</v>
       </c>
-      <c r="D47" s="32">
+      <c r="D47" s="31">
         <v>9</v>
       </c>
-      <c r="E47" s="32">
+      <c r="E47" s="31">
         <v>2.1</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="32">
+      <c r="B48" s="31">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C48" s="32">
+      <c r="C48" s="31">
         <v>8.5</v>
       </c>
-      <c r="D48" s="32">
+      <c r="D48" s="31">
         <v>8.9</v>
       </c>
-      <c r="E48" s="32">
+      <c r="E48" s="31">
         <v>1.9</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="32">
+      <c r="B49" s="31">
         <v>0.253</v>
       </c>
-      <c r="C49" s="32">
+      <c r="C49" s="31">
         <v>9.1</v>
       </c>
-      <c r="D49" s="32">
+      <c r="D49" s="31">
         <v>10</v>
       </c>
-      <c r="E49" s="32">
+      <c r="E49" s="31">
         <v>2.1</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="32">
+      <c r="B50" s="31">
         <v>0.32900000000000001</v>
       </c>
-      <c r="C50" s="32">
+      <c r="C50" s="31">
         <v>8.8000000000000007</v>
       </c>
-      <c r="D50" s="32">
+      <c r="D50" s="31">
         <v>10</v>
       </c>
-      <c r="E50" s="32">
+      <c r="E50" s="31">
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="32">
+      <c r="B51" s="31">
         <v>0.26700000000000002</v>
       </c>
-      <c r="C51" s="32">
+      <c r="C51" s="31">
         <v>9.6</v>
       </c>
-      <c r="D51" s="32">
+      <c r="D51" s="31">
         <v>10</v>
       </c>
-      <c r="E51" s="32">
+      <c r="E51" s="31">
         <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="32">
+      <c r="B52" s="31">
         <v>0.254</v>
       </c>
-      <c r="C52" s="32">
+      <c r="C52" s="31">
         <v>9.4</v>
       </c>
-      <c r="D52" s="32">
+      <c r="D52" s="31">
         <v>9.5</v>
       </c>
-      <c r="E52" s="32">
+      <c r="E52" s="31">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="33">
+      <c r="B53" s="32">
         <v>0.24</v>
       </c>
-      <c r="C53" s="33">
+      <c r="C53" s="32">
         <v>8.8000000000000007</v>
       </c>
-      <c r="D53" s="33">
+      <c r="D53" s="32">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E53" s="33">
+      <c r="E53" s="32">
         <v>2.6</v>
       </c>
     </row>
@@ -22239,312 +24122,312 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD661B37-D27A-4799-8CC8-98F6490B983D}">
   <dimension ref="B1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B1" s="32">
+      <c r="B1" s="31">
         <v>34.6</v>
       </c>
-      <c r="C1" s="34">
+      <c r="C1" s="33">
         <v>19.100000000000001</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="31">
         <v>0.50600000000000001</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="32">
+      <c r="B2" s="31">
         <v>23.2</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="31">
         <v>14.4</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <v>0.50600000000000001</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="32">
+      <c r="B3" s="31">
         <v>19.2</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="31">
         <v>13.7</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="31">
         <v>0.19500000000000001</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="32">
+      <c r="B4" s="31">
         <v>16.7</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="31">
         <v>12.8</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <v>0.19500000000000001</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <v>17.399999999999999</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="31">
         <v>11.4</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="31">
         <v>0.254</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <v>17.3</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <v>11.3</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <v>0.27</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <v>15.6</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <v>17.2</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <v>0.29399999999999998</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <v>18.7</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>13.3</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>0.246</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="34"/>
-      <c r="C9" s="32">
+      <c r="B9" s="33"/>
+      <c r="C9" s="31">
         <v>12.4</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <v>0.35499999999999998</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="32"/>
-      <c r="C10" s="32">
+      <c r="B10" s="31"/>
+      <c r="C10" s="31">
         <v>11.1</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <v>0.26700000000000002</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="32"/>
-      <c r="C11" s="32">
+      <c r="B11" s="31"/>
+      <c r="C11" s="31">
         <v>12.1</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <v>0.219</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="32"/>
-      <c r="C12" s="32">
+      <c r="B12" s="31"/>
+      <c r="C12" s="31">
         <v>10.3</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="31">
         <v>0.24</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="32"/>
-      <c r="C13" s="32">
+      <c r="B13" s="31"/>
+      <c r="C13" s="31">
         <v>9.8000000000000007</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="32"/>
-      <c r="C14" s="32">
+      <c r="B14" s="31"/>
+      <c r="C14" s="31">
         <v>8.6999999999999993</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="31">
         <v>0.253</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="32"/>
-      <c r="C15" s="32">
+      <c r="B15" s="31"/>
+      <c r="C15" s="31">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="31">
         <v>0.32900000000000001</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="32"/>
-      <c r="C16" s="32">
+      <c r="B16" s="31"/>
+      <c r="C16" s="31">
         <v>7.8</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <v>0.26700000000000002</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="32"/>
-      <c r="C17" s="32">
+      <c r="B17" s="31"/>
+      <c r="C17" s="31">
         <v>9.1999999999999993</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <v>0.254</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="32"/>
-      <c r="C18" s="32">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31">
         <v>9.1999999999999993</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="32">
         <v>0.24</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="32"/>
-      <c r="C19" s="32">
+      <c r="B19" s="31"/>
+      <c r="C19" s="31">
         <v>7.9</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="32"/>
-      <c r="C20" s="32">
+      <c r="B20" s="31"/>
+      <c r="C20" s="31">
         <v>7.4</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="32"/>
-      <c r="C21" s="32">
+      <c r="B21" s="31"/>
+      <c r="C21" s="31">
         <v>10.4</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="32"/>
-      <c r="C22" s="33">
+      <c r="B22" s="31"/>
+      <c r="C22" s="32">
         <v>10.4</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="33"/>
-      <c r="C30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="31"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="32"/>
-      <c r="C40" s="33"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="32"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="32"/>
+      <c r="B41" s="31"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="32"/>
+      <c r="B42" s="31"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="32"/>
+      <c r="B43" s="31"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="32"/>
+      <c r="B44" s="31"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="32"/>
+      <c r="B45" s="31"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="32"/>
+      <c r="B46" s="31"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="32"/>
+      <c r="B47" s="31"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="33"/>
+      <c r="B48" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>